<commit_message>
Update HRT Schedule to CSV Converter 1.1.xlsx
</commit_message>
<xml_diff>
--- a/HRT Schedule to CSV Converter 1.1.xlsx
+++ b/HRT Schedule to CSV Converter 1.1.xlsx
@@ -83,21 +83,20 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">1. You will have to modify only PINK CELLS - the whole rest will adjust automatically 
+    <t>1. You will have to modify only PINK CELLS - the whole rest will adjust automatically
 2. Paste ROW 2 of Sharepoint HireRight Schedule into B1 cell (1st RED MARKER)
-3. Paste your PERSONAL ROW of Sharepoint HireRight Schedule into B2 cell (2nd RED MARKER)
-4. Delete all WORKDAYS and DAYS OFF columns in INPUT sheet - it's crucial
-5. Set DATE OF THE FIRST DAY of your schedule (3rd RED MARKER)
-6. Make sure you align dates, day names and shifts
-7. You can change names of the events using italic values on the left
-8. Open OUTPUT sheet
-9. Export OUTPUT sheet using FILE / DOWNLOAD / COMMA-SEPARATED VALUES (.CSV)
+3. Paste your PERSONAL ROW of Sharepoint HireRight Schedule into the B2 cell (2nd RED MARKER)
+4. Delete all WORKDAYS / DAYS OFF columns in the INPUT sheet - it's crucial
+5. Set the DATE OF THE FIRST DAY of your schedule (3rd RED MARKER)
+6. Make sure you align dates, day names, and shifts
+7. You can change the names of the events using italic values on the left
+8. Open the OUTPUT sheet
+9. Export the OUTPUT sheet using FILE / DOWNLOAD / COMMA-SEPARATED VALUES (.CSV)
 10. You can import .CSV file to e.g. Google Calendar by using SETTINGS / IMPORT &amp; EXPORT / 
 SELECT FILE FROM YOUR COMPUTER / ADD TO CALENDAR / IMPORT
-11. It's very good idea to import .CSV schedule to the new calendar, not adding it to existing one
+11. It's a very good idea to import the .CSV schedule to the new calendar, not add it to the existing one
 12. By using the schedule in your preferable calendar app you can use various automation scripts
-13. You can experiment and modify cells but be aware that changes in OUTPUT sheet can mess up your .CSV
-</t>
+13. You can experiment and modify cells but be aware that changes in the OUTPUT sheet can mess up your .CSV</t>
   </si>
   <si>
     <t>Shift 1 Title</t>
@@ -1935,13 +1934,13 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E13:L23"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E13:L23"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>